<commit_message>
some more testCases for Admin and PIM
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,34 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java-learning\Automation Testing\com.crm.orangeHRMproject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5164B398-CD65-4360-8259-9C68DD5E8E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28526FA-7B9A-4CEF-8F79-6564D8F25C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{98210E40-9D2C-41ED-8F31-7AAE7EEF21CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{98210E40-9D2C-41ED-8F31-7AAE7EEF21CD}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="url" sheetId="2" r:id="rId2"/>
+    <sheet name="admin" sheetId="3" r:id="rId3"/>
+    <sheet name="pim" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>testcase</t>
   </si>
@@ -64,13 +57,157 @@
     <t>admins</t>
   </si>
   <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/dashboard/index</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewSystemUsers</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/viewEmployeeList</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/leave/viewLeaveList</t>
+  </si>
+  <si>
+    <t>Leave</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/time/viewEmployeeTimesheet</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
     <t>header</t>
   </si>
   <si>
-    <t>User Management</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
+    <t>job</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewJobTitleList</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewPayGrades</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/employmentStatus</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/jobCategory</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/workShift</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewOrganizationGeneralInformation</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewLocations</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewCompanyStructure</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewSkills</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewEducation</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewLicenses</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewLanguages</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/membership</t>
+  </si>
+  <si>
+    <t>Nationalities</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/nationality</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/addTheme</t>
+  </si>
+  <si>
+    <t>Corporate Branding</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/listMailConfiguration</t>
+  </si>
+  <si>
+    <t>Configurations</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewEmailNotification</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/localization</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/languagePackage</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/viewModules</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/openIdProvider</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/registerOAuthClient</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/admin/ldapConfiguration</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/configurePim</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/listCustomFields</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/pimCsvImport</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/viewReportingMethods</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/viewTerminationReasons</t>
+  </si>
+  <si>
+    <t>Employee List</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/addEmployee</t>
+  </si>
+  <si>
+    <t>Add Employee</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/viewDefinedPredefinedReports</t>
+  </si>
+  <si>
+    <t>Reports</t>
   </si>
 </sst>
 </file>
@@ -86,16 +223,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7.5"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFE3E3E3"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,20 +254,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C430E5-BDF2-448B-9458-0900B493B8A1}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,33 +669,303 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B1CF66-6867-45F8-8E58-4208C1665023}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="76.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3386AAC2-DDF3-41CD-83DE-80EC03735753}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{8B39BB2F-3F6F-4D50-AC0F-FA08BF74AEDB}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{46257040-937A-430E-8070-3E2E41D7D21E}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{5ED117AA-C34C-4923-AF76-33EF1D7F8C7F}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{02B813B5-81BE-4A7E-8D62-CCE94C2C13AC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F985CF-C7C3-4E8D-BAAE-F6362945504D}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView zoomScale="139" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="74.88671875" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+    <col min="3" max="3" width="77.109375" customWidth="1"/>
+    <col min="4" max="4" width="78.109375" customWidth="1"/>
+    <col min="5" max="5" width="87.21875" customWidth="1"/>
+    <col min="6" max="6" width="56.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CA9747CA-1B6D-47EC-93FD-FD374F68248B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{18B234B9-9DD1-47A0-A5A4-AB98E9F62935}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{19F4A492-BA2B-4841-BC58-6F39906A9C60}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{FBCC0880-B553-47DA-B016-1BFDFD3B2024}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{F1ADA8C0-D80F-488B-9974-8D7826DD6AAD}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{D177D958-12D3-471C-A0BD-C7E550756CE4}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{BB8C7559-1B59-4ACE-83FD-D135E950F0DF}"/>
+    <hyperlink ref="B4" r:id="rId8" xr:uid="{F36019BC-6A0B-44BE-B208-EEE0E1126716}"/>
+    <hyperlink ref="C2" r:id="rId9" xr:uid="{825EF24F-8E32-4352-B8A3-C286DA572A81}"/>
+    <hyperlink ref="C3" r:id="rId10" xr:uid="{A7C4BA9D-9402-4969-95FC-B8C45325298C}"/>
+    <hyperlink ref="C5" r:id="rId11" xr:uid="{D85BBC94-BECD-4EDD-9BE3-623ABBD69174}"/>
+    <hyperlink ref="C6" r:id="rId12" xr:uid="{D84294DE-051D-4ACB-85E9-94D2B153C48B}"/>
+    <hyperlink ref="C4" r:id="rId13" xr:uid="{65F16D00-6996-4A4B-98A4-F06B0DCD9B2F}"/>
+    <hyperlink ref="D2" r:id="rId14" xr:uid="{8F6A652E-24F3-456E-94CC-552FE15FA2F0}"/>
+    <hyperlink ref="E2" r:id="rId15" xr:uid="{411B0DC3-E978-4438-AB7D-53D73994F884}"/>
+    <hyperlink ref="F2" r:id="rId16" xr:uid="{488F4A69-723F-4DF8-9E8B-D298403455A5}"/>
+    <hyperlink ref="F4" r:id="rId17" xr:uid="{5F9BBD95-8F33-4B15-B9A4-C034A8FB9039}"/>
+    <hyperlink ref="F3" r:id="rId18" xr:uid="{82E24DE2-CCAD-49EB-AB84-91B80FD83C33}"/>
+    <hyperlink ref="F6" r:id="rId19" xr:uid="{3CAC3C2A-A3F5-40F8-BE63-02D2736EBD81}"/>
+    <hyperlink ref="F8" r:id="rId20" xr:uid="{A20F1DA8-94D2-471A-AFA7-901BA0DA0CFE}"/>
+    <hyperlink ref="F5" r:id="rId21" xr:uid="{D1A0B5F3-D97C-4365-AB08-53D7AC20CFE0}"/>
+    <hyperlink ref="F7" r:id="rId22" xr:uid="{88ACA520-210F-4E47-8DE7-3D8A71775B43}"/>
+    <hyperlink ref="F9" r:id="rId23" xr:uid="{899ECE53-E993-412E-86ED-255F70587982}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5B139A-7485-45A6-960C-17433109B999}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="76.44140625" customWidth="1"/>
+    <col min="2" max="2" width="70.88671875" customWidth="1"/>
+    <col min="3" max="3" width="66" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{131F21A6-CBCF-4F86-B1EE-20DF35D97413}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{015DE2E0-B855-4BDA-906C-91A5F060F945}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A49D4C56-9BCB-4F11-AFA6-216A61580745}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{1F09642A-FB78-4195-A340-6E307F1C6D18}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{7D957D24-0E1B-448A-8C59-71EFA3C7542E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>